<commit_message>
Add arrows to Relation Model
I have also created InProgress folders
</commit_message>
<xml_diff>
--- a/design/data-structure/RelationModel.xlsx
+++ b/design/data-structure/RelationModel.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miro\Documents\GitHub\prj1-2020-group-prj1-2020-15\design\data-structure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/GitHub/prj1-2020-group-prj1-2020-15/design/data-structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A436572F-0696-4D56-A342-9BCFC472559E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4FDC8D-64AA-0946-A243-047183ACA1D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12156" yWindow="684" windowWidth="17280" windowHeight="8964" xr2:uid="{FAADFD9B-3F1E-4BA2-A717-100F9F568774}"/>
+    <workbookView xWindow="12160" yWindow="680" windowWidth="17280" windowHeight="8960" activeTab="1" xr2:uid="{FAADFD9B-3F1E-4BA2-A717-100F9F568774}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Draft" sheetId="1" r:id="rId1"/>
+    <sheet name="WithArrows" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>USER</t>
   </si>
@@ -124,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,16 +141,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -157,13 +184,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,6 +233,1391 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBBC2C48-32E4-FA4C-BD9E-2AF2A5EDA733}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2006600" y="787400"/>
+          <a:ext cx="0" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98FBA58-61B2-BA44-87B8-9C71478328A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1993900" y="1143000"/>
+          <a:ext cx="7150100" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B205A18-31F4-234C-B510-CC925C51EBDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1854200" y="2057400"/>
+          <a:ext cx="0" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6C9F4D-FCAB-6944-949F-5416B83615D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1854200" y="4597400"/>
+          <a:ext cx="0" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6351BD8B-C886-304F-A886-3FC4B5F981F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1879600" y="7137400"/>
+          <a:ext cx="0" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23D61B87-D1A8-FA48-A998-E6897409D51F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7835900" y="6210300"/>
+          <a:ext cx="1308100" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C912C5A-864B-7145-BDC7-82D9CCEDBC56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9131300" y="1130300"/>
+          <a:ext cx="0" cy="5092700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A12EEB85-5DB2-5340-9255-18B116E1B648}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7854950" y="5848350"/>
+          <a:ext cx="0" cy="374650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBFE8A58-D4E0-CF4C-89D6-9F3BAA7AD0DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6667500" y="4940300"/>
+          <a:ext cx="2298700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2B408D-2897-0A4D-AA1B-1A8639EFD079}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6686550" y="4578350"/>
+          <a:ext cx="0" cy="374650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>517663</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6902</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>522006</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133685</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B72C332-C244-8F4D-99C8-46EEE367C2CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8963163" y="1276902"/>
+          <a:ext cx="4343" cy="3682783"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>537231</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E1231BD-9DCF-2449-98A9-9CBF49731361}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1701800" y="1282560"/>
+          <a:ext cx="7280931" cy="140"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD3AB49B-EDB2-3947-BAE4-DED29E434BDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1714500" y="774700"/>
+          <a:ext cx="0" cy="518160"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02F80F86-E5A6-8041-A9C4-F6A3871D5002}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="787400" y="2400300"/>
+          <a:ext cx="1079500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA88C6A9-C94C-4C45-8C1E-9BA8947CB4A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="4953000"/>
+          <a:ext cx="876300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>977900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC6EEAA3-0E30-F341-87CB-AE6ED548BE28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="977900" y="7493000"/>
+          <a:ext cx="914400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>996950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15B6B01D-569D-C24F-93AD-DA0F2373A6FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="996950" y="6337300"/>
+          <a:ext cx="6350" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{757450A5-69CF-AA4F-B95B-559ECA535A7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="6350000"/>
+          <a:ext cx="5765800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56C54042-417B-424B-9B8B-628FFF1FF355}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6737350" y="5854700"/>
+          <a:ext cx="0" cy="508000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFF89EEE-47A4-604A-B43F-AF3EBBB35C96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5499100" y="5848350"/>
+          <a:ext cx="0" cy="273050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A93D9C2-9934-6049-A72A-5BE5B70BA8B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1003300" y="4933950"/>
+          <a:ext cx="0" cy="1187450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A9EAC2F-196C-1D43-ADE9-9A8D85F5861E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="6108700"/>
+          <a:ext cx="4521200" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD6241B-4F1A-3941-8828-6783706E4491}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="787400" y="2381250"/>
+          <a:ext cx="0" cy="5365750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AAC8F96-DC01-5A41-A7DD-A0A2EBE9B685}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="774700" y="7721600"/>
+          <a:ext cx="9537700" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{608BFB6B-6292-4B4B-8877-B32D316C7F8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10299700" y="7137400"/>
+          <a:ext cx="0" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,22 +1919,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CED035B-130F-4EFB-95EA-4039A48DBA16}">
   <dimension ref="B3:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
@@ -518,12 +1957,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
@@ -540,12 +1979,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -553,12 +1992,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
@@ -575,12 +2014,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -600,12 +2039,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
@@ -635,4 +2074,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8557DB-FF7B-F64F-AB1D-9C2FB90D9680}">
+  <dimension ref="B2:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="15.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Database script and data input examples
</commit_message>
<xml_diff>
--- a/design/data-structure/RelationModel.xlsx
+++ b/design/data-structure/RelationModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/GitHub/prj1-2020-group-prj1-2020-15/design/data-structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCDE824-38D9-BA4E-8FBA-436016FD3E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE951D45-25E3-DC40-B325-EAEDCCB271AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15840" yWindow="460" windowWidth="12960" windowHeight="16460" activeTab="1" xr2:uid="{FAADFD9B-3F1E-4BA2-A717-100F9F568774}"/>
+    <workbookView xWindow="3300" yWindow="600" windowWidth="12960" windowHeight="16460" activeTab="1" xr2:uid="{FAADFD9B-3F1E-4BA2-A717-100F9F568774}"/>
   </bookViews>
   <sheets>
     <sheet name="Draft" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>USER</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>EventNumber</t>
-  </si>
-  <si>
-    <t>CMail</t>
   </si>
   <si>
     <t>E_Name</t>
@@ -262,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -285,11 +282,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,6 +308,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -323,117 +335,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBBC2C48-32E4-FA4C-BD9E-2AF2A5EDA733}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2006600" y="787400"/>
-          <a:ext cx="0" cy="365760"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98FBA58-61B2-BA44-87B8-9C71478328A8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1993900" y="1143000"/>
-          <a:ext cx="7150100" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -583,171 +484,6 @@
             <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Connector 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23D61B87-D1A8-FA48-A998-E6897409D51F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7835900" y="6210300"/>
-          <a:ext cx="1308100" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Straight Connector 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C912C5A-864B-7145-BDC7-82D9CCEDBC56}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9131300" y="1130300"/>
-          <a:ext cx="0" cy="5092700"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A12EEB85-5DB2-5340-9255-18B116E1B648}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7854950" y="5848350"/>
-          <a:ext cx="0" cy="374650"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2167,7 +1903,7 @@
   <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2182,7 +1918,7 @@
     </row>
     <row r="3" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>30</v>
@@ -2210,7 +1946,7 @@
     </row>
     <row r="8" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>35</v>
@@ -2227,12 +1963,12 @@
     </row>
     <row r="12" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>39</v>
@@ -2240,7 +1976,7 @@
     </row>
     <row r="17" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2264,6 +2000,7 @@
       <c r="B22" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
@@ -2273,7 +2010,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>42</v>
@@ -2281,13 +2018,11 @@
       <c r="F23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="G23" s="7"/>
     </row>
     <row r="27" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2295,22 +2030,22 @@
         <v>23</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>